<commit_message>
dashboard updates + model updates
</commit_message>
<xml_diff>
--- a/Commodities/Cameco.xlsx
+++ b/Commodities/Cameco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Commodities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4308CB-B0F9-2646-BF71-91A76E67F69F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A637E6-190B-3B43-ACCC-DEFEF4604634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2781,9 +2781,10 @@
       <sheetName val="Industrials"/>
       <sheetName val="Commodities"/>
       <sheetName val="US Treasury Bonds"/>
-      <sheetName val="Full Portfolio"/>
+      <sheetName val="Growth"/>
       <sheetName val="Full Portfolio (Concentrated)"/>
-      <sheetName val="Growth"/>
+      <sheetName val="Value"/>
+      <sheetName val="Concentrated"/>
       <sheetName val="Watchlist"/>
       <sheetName val="Wide Moats"/>
       <sheetName val="Sheet2"/>
@@ -2802,7 +2803,7 @@
       <sheetData sheetId="6">
         <row r="8">
           <cell r="C8">
-            <v>4.9020000000000001E-2</v>
+            <v>4.9880000000000008E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -2816,6 +2817,7 @@
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2943,11 +2945,11 @@
     <v>Powered by Refinitiv</v>
     <v>56.87</v>
     <v>28.98</v>
-    <v>0.91520000000000001</v>
-    <v>0.71</v>
-    <v>1.3680000000000001E-2</v>
-    <v>0</v>
-    <v>0</v>
+    <v>0.91990000000000005</v>
+    <v>-0.25</v>
+    <v>-4.7520000000000001E-3</v>
+    <v>0.53</v>
+    <v>1.0121999999999999E-2</v>
     <v>CAD</v>
     <v>Cameco Corporation is a Canada-based company engaged in providing uranium fuel to generate clean, reliable baseload electricity around the globe. The Company also offers nuclear fuel processing services, refinery services and manufactures fuel assemblies and reactor components. It operates through two segments: uranium and fuel services. The uranium segment is involved in the exploration for, mining, milling, purchase and sale of uranium concentrate. The fuel services segment is involved in the refining, conversion and fabrication of uranium concentrate and the purchase and sale of conversion services. Its uranium projects include Millennium, Yeelirrie, and Kintyre. The Cree Extension-Millennium project is a Cameco-operated joint venture located in the southeastern portion of Canada's Athabasca Basin. The Yeelirrie deposit is located approximately 650 kilometer (Km) northeast of Perth and approximately 750 km south of the Company’s Kintyre project.</v>
     <v>2424</v>
@@ -2955,25 +2957,25 @@
     <v>XTSE</v>
     <v>XTSE</v>
     <v>2121 11th St W, SASKATOON, SK, S7M 1J3 CA</v>
-    <v>53.38</v>
+    <v>53.09</v>
     <v>Uranium</v>
     <v>Stock</v>
-    <v>45218.844108796293</v>
+    <v>45219.844224537039</v>
     <v>0</v>
-    <v>50.75</v>
-    <v>22625050000</v>
+    <v>51.36</v>
+    <v>22715741972</v>
     <v>CAMECO CORPORATION</v>
     <v>CAMECO CORPORATION</v>
-    <v>51.77</v>
-    <v>239.87</v>
-    <v>51.9</v>
+    <v>52.89</v>
+    <v>243.15</v>
     <v>52.61</v>
-    <v>52.61</v>
+    <v>52.36</v>
+    <v>52.89</v>
     <v>433837700</v>
     <v>CCO</v>
     <v>CAMECO CORPORATION (XTSE:CCO)</v>
-    <v>1373429</v>
-    <v>1208660</v>
+    <v>953527</v>
+    <v>1172860</v>
     <v>1997</v>
   </rv>
   <rv s="2">
@@ -3562,7 +3564,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="AC88" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AJ85" sqref="AJ85"/>
+      <selection pane="bottomRight" activeCell="AI95" sqref="AI95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5376,15 +5378,15 @@
       </c>
       <c r="AL16" s="32">
         <f>AM102/AE3</f>
-        <v>12.111891683257468</v>
+        <v>12.160441911495859</v>
       </c>
       <c r="AM16" s="32">
         <f>AM102/AE28</f>
-        <v>253.12758720995279</v>
+        <v>254.14224309145018</v>
       </c>
       <c r="AN16" s="33">
         <f>AM102/AE107</f>
-        <v>140.38961522471595</v>
+        <v>140.9523636408764</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -5704,15 +5706,15 @@
       </c>
       <c r="AL19" s="32">
         <f>AM102/AF3</f>
-        <v>9.1747972424979718</v>
+        <v>9.2115741978913217</v>
       </c>
       <c r="AM19" s="32">
         <f>AM102/AF28</f>
-        <v>76.050588235294114</v>
+        <v>76.355435200000002</v>
       </c>
       <c r="AN19" s="33">
         <f>AM102/AF107</f>
-        <v>95.063235294117646</v>
+        <v>95.444293999999999</v>
       </c>
     </row>
     <row r="20" spans="1:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -6081,11 +6083,11 @@
       </c>
       <c r="AM22" s="42">
         <f>(-1*AE98)/AM102</f>
-        <v>2.2936965885158264E-3</v>
+        <v>2.284539068279922E-3</v>
       </c>
       <c r="AN22" s="41">
         <f>AF107/AM102</f>
-        <v>1.0519313769472332E-2</v>
+        <v>1.0477315699983071E-2</v>
       </c>
     </row>
     <row r="23" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -13363,7 +13365,7 @@
       </c>
       <c r="AM95" s="56">
         <f>'[1]US Treasury Bonds'!$C$8</f>
-        <v>4.9020000000000001E-2</v>
+        <v>4.9880000000000008E-2</v>
       </c>
     </row>
     <row r="96" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -13471,7 +13473,7 @@
       </c>
       <c r="AM96" s="57" cm="1">
         <f t="array" ref="AM96">_FV(A1,"Beta")</f>
-        <v>0.91520000000000001</v>
+        <v>0.91990000000000005</v>
       </c>
     </row>
     <row r="97" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -13686,7 +13688,7 @@
       </c>
       <c r="AM98" s="55">
         <f>(AM95)+((AM96)*(AM97-AM95))</f>
-        <v>8.1033696000000002E-2</v>
+        <v>8.1266988000000012E-2</v>
       </c>
     </row>
     <row r="99" spans="1:39" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -14007,7 +14009,7 @@
       </c>
       <c r="AM101" s="55">
         <f>AM100/AM104</f>
-        <v>4.2206328409261688E-2</v>
+        <v>4.204490569573343E-2</v>
       </c>
     </row>
     <row r="102" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -14115,7 +14117,7 @@
       </c>
       <c r="AM102" s="58" cm="1">
         <f t="array" ref="AM102">_FV(A1,"Market cap",TRUE)</f>
-        <v>22625050000</v>
+        <v>22715741972</v>
       </c>
     </row>
     <row r="103" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -14223,7 +14225,7 @@
       </c>
       <c r="AM103" s="55">
         <f>AM102/AM104</f>
-        <v>0.95779367159073836</v>
+        <v>0.95795509430426662</v>
       </c>
     </row>
     <row r="104" spans="1:39" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -14333,7 +14335,7 @@
       </c>
       <c r="AM104" s="59">
         <f>AM100+AM102</f>
-        <v>23622050000</v>
+        <v>23712741972</v>
       </c>
     </row>
     <row r="105" spans="1:39" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -14634,7 +14636,7 @@
       </c>
       <c r="AM106" s="60">
         <f>(AM101*AM93)+(AM103*AM98)</f>
-        <v>8.0690201459527142E-2</v>
+        <v>8.0914998451780212E-2</v>
       </c>
     </row>
     <row r="107" spans="1:39" ht="19" x14ac:dyDescent="0.25">
@@ -14764,7 +14766,7 @@
       <c r="AI108" s="44"/>
       <c r="AJ108" s="47">
         <f>AJ107*(1+AM108)/(AM109-AM108)</f>
-        <v>18957553974.1451</v>
+        <v>18881338267.592979</v>
       </c>
       <c r="AK108" s="48" t="s">
         <v>144</v>
@@ -14795,7 +14797,7 @@
       </c>
       <c r="AJ109" s="47">
         <f>AJ108+AJ107</f>
-        <v>19987553974.1451</v>
+        <v>19911338267.592979</v>
       </c>
       <c r="AK109" s="48" t="s">
         <v>142</v>
@@ -14805,7 +14807,7 @@
       </c>
       <c r="AM109" s="39">
         <f>AM106</f>
-        <v>8.0690201459527142E-2</v>
+        <v>8.0914998451780212E-2</v>
       </c>
     </row>
     <row r="110" spans="1:39" ht="19" x14ac:dyDescent="0.2">
@@ -14826,7 +14828,7 @@
       </c>
       <c r="AG111" s="58">
         <f>NPV(AM109,AF109,AG109,AH109,AI109,AJ109)</f>
-        <v>15623444933.744766</v>
+        <v>15556494977.504606</v>
       </c>
       <c r="AH111" s="49"/>
       <c r="AI111" s="49"/>
@@ -14871,7 +14873,7 @@
       </c>
       <c r="AG114" s="58">
         <f>AG111+AG112-AG113</f>
-        <v>16669292933.744766</v>
+        <v>16602342977.504608</v>
       </c>
       <c r="AH114" s="49"/>
       <c r="AI114" s="49"/>
@@ -14901,7 +14903,7 @@
       </c>
       <c r="AG116" s="66">
         <f>AG114/AG115</f>
-        <v>39.806714923627766</v>
+        <v>39.646836647278903</v>
       </c>
       <c r="AH116" s="49"/>
       <c r="AI116" s="49"/>
@@ -14916,7 +14918,7 @@
       </c>
       <c r="AG117" s="67" cm="1">
         <f t="array" ref="AG117">_FV(A1,"Price")</f>
-        <v>52.61</v>
+        <v>52.36</v>
       </c>
       <c r="AH117" s="49"/>
       <c r="AI117" s="49"/>
@@ -14931,7 +14933,7 @@
       </c>
       <c r="AG118" s="68">
         <f>AG116/AG117-1</f>
-        <v>-0.24336219495100231</v>
+        <v>-0.24280296701148008</v>
       </c>
       <c r="AH118" s="49"/>
       <c r="AI118" s="49"/>

</xml_diff>

<commit_message>
Lots of new models / changes
</commit_message>
<xml_diff>
--- a/Commodities/Cameco.xlsx
+++ b/Commodities/Cameco.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Commodities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A637E6-190B-3B43-ACCC-DEFEF4604634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28203BDD-ACDF-7F40-8EE6-1838E15C6615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2777,6 +2777,7 @@
       <sheetName val="Software"/>
       <sheetName val="Hardware"/>
       <sheetName val="Consumer"/>
+      <sheetName val="Financials"/>
       <sheetName val="Healthcare"/>
       <sheetName val="Industrials"/>
       <sheetName val="Commodities"/>
@@ -2800,14 +2801,14 @@
       <sheetData sheetId="3"/>
       <sheetData sheetId="4"/>
       <sheetData sheetId="5"/>
-      <sheetData sheetId="6">
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7">
         <row r="8">
           <cell r="C8">
-            <v>4.9880000000000008E-2</v>
+            <v>4.845E-2</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="7"/>
       <sheetData sheetId="8"/>
       <sheetData sheetId="9"/>
       <sheetData sheetId="10"/>
@@ -2818,6 +2819,7 @@
       <sheetData sheetId="15"/>
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2945,11 +2947,11 @@
     <v>Powered by Refinitiv</v>
     <v>56.87</v>
     <v>28.98</v>
-    <v>0.91990000000000005</v>
-    <v>-0.25</v>
-    <v>-4.7520000000000001E-3</v>
-    <v>0.53</v>
-    <v>1.0121999999999999E-2</v>
+    <v>0.92120000000000002</v>
+    <v>-0.38</v>
+    <v>-7.1660000000000005E-3</v>
+    <v>0</v>
+    <v>0</v>
     <v>CAD</v>
     <v>Cameco Corporation is a Canada-based company engaged in providing uranium fuel to generate clean, reliable baseload electricity around the globe. The Company also offers nuclear fuel processing services, refinery services and manufactures fuel assemblies and reactor components. It operates through two segments: uranium and fuel services. The uranium segment is involved in the exploration for, mining, milling, purchase and sale of uranium concentrate. The fuel services segment is involved in the refining, conversion and fabrication of uranium concentrate and the purchase and sale of conversion services. Its uranium projects include Millennium, Yeelirrie, and Kintyre. The Cree Extension-Millennium project is a Cameco-operated joint venture located in the southeastern portion of Canada's Athabasca Basin. The Yeelirrie deposit is located approximately 650 kilometer (Km) northeast of Perth and approximately 750 km south of the Company’s Kintyre project.</v>
     <v>2424</v>
@@ -2957,25 +2959,25 @@
     <v>XTSE</v>
     <v>XTSE</v>
     <v>2121 11th St W, SASKATOON, SK, S7M 1J3 CA</v>
-    <v>53.09</v>
+    <v>53.63</v>
     <v>Uranium</v>
     <v>Stock</v>
-    <v>45219.844224537039</v>
+    <v>45226.833333333336</v>
     <v>0</v>
-    <v>51.36</v>
-    <v>22715741972</v>
+    <v>52.465000000000003</v>
+    <v>22904310000</v>
     <v>CAMECO CORPORATION</v>
     <v>CAMECO CORPORATION</v>
-    <v>52.89</v>
-    <v>243.15</v>
-    <v>52.61</v>
-    <v>52.36</v>
-    <v>52.89</v>
+    <v>53.51</v>
+    <v>243.33</v>
+    <v>53.03</v>
+    <v>52.65</v>
+    <v>52.65</v>
     <v>433837700</v>
     <v>CCO</v>
     <v>CAMECO CORPORATION (XTSE:CCO)</v>
-    <v>953527</v>
-    <v>1172860</v>
+    <v>697591</v>
+    <v>1083790</v>
     <v>1997</v>
   </rv>
   <rv s="2">
@@ -3561,10 +3563,10 @@
   <dimension ref="A1:AN119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AC88" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AB95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AI95" sqref="AI95"/>
+      <selection pane="bottomRight" activeCell="AF121" sqref="AF121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5378,15 +5380,15 @@
       </c>
       <c r="AL16" s="32">
         <f>AM102/AE3</f>
-        <v>12.160441911495859</v>
+        <v>12.261388231175218</v>
       </c>
       <c r="AM16" s="32">
         <f>AM102/AE28</f>
-        <v>254.14224309145018</v>
+        <v>256.2519299187756</v>
       </c>
       <c r="AN16" s="33">
         <f>AM102/AE107</f>
-        <v>140.9523636408764</v>
+        <v>142.12243808909213</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -5706,15 +5708,15 @@
       </c>
       <c r="AL19" s="32">
         <f>AM102/AF3</f>
-        <v>9.2115741978913217</v>
+        <v>9.2880413625304143</v>
       </c>
       <c r="AM19" s="32">
         <f>AM102/AF28</f>
-        <v>76.355435200000002</v>
+        <v>76.989277310924365</v>
       </c>
       <c r="AN19" s="33">
         <f>AM102/AF107</f>
-        <v>95.444293999999999</v>
+        <v>96.236596638655456</v>
       </c>
     </row>
     <row r="20" spans="1:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -6083,11 +6085,11 @@
       </c>
       <c r="AM22" s="42">
         <f>(-1*AE98)/AM102</f>
-        <v>2.284539068279922E-3</v>
+        <v>2.2657307729418612E-3</v>
       </c>
       <c r="AN22" s="41">
         <f>AF107/AM102</f>
-        <v>1.0477315699983071E-2</v>
+        <v>1.039105740360657E-2</v>
       </c>
     </row>
     <row r="23" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -13365,7 +13367,7 @@
       </c>
       <c r="AM95" s="56">
         <f>'[1]US Treasury Bonds'!$C$8</f>
-        <v>4.9880000000000008E-2</v>
+        <v>4.845E-2</v>
       </c>
     </row>
     <row r="96" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -13473,7 +13475,7 @@
       </c>
       <c r="AM96" s="57" cm="1">
         <f t="array" ref="AM96">_FV(A1,"Beta")</f>
-        <v>0.91990000000000005</v>
+        <v>0.92120000000000002</v>
       </c>
     </row>
     <row r="97" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -13688,7 +13690,7 @@
       </c>
       <c r="AM98" s="55">
         <f>(AM95)+((AM96)*(AM97-AM95))</f>
-        <v>8.1266988000000012E-2</v>
+        <v>8.1198660000000006E-2</v>
       </c>
     </row>
     <row r="99" spans="1:39" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -14009,7 +14011,7 @@
       </c>
       <c r="AM101" s="55">
         <f>AM100/AM104</f>
-        <v>4.204490569573343E-2</v>
+        <v>4.1713194799782943E-2</v>
       </c>
     </row>
     <row r="102" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -14117,7 +14119,7 @@
       </c>
       <c r="AM102" s="58" cm="1">
         <f t="array" ref="AM102">_FV(A1,"Market cap",TRUE)</f>
-        <v>22715741972</v>
+        <v>22904310000</v>
       </c>
     </row>
     <row r="103" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -14225,7 +14227,7 @@
       </c>
       <c r="AM103" s="55">
         <f>AM102/AM104</f>
-        <v>0.95795509430426662</v>
+        <v>0.95828680520021703</v>
       </c>
     </row>
     <row r="104" spans="1:39" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -14335,7 +14337,7 @@
       </c>
       <c r="AM104" s="59">
         <f>AM100+AM102</f>
-        <v>23712741972</v>
+        <v>23901310000</v>
       </c>
     </row>
     <row r="105" spans="1:39" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -14636,7 +14638,7 @@
       </c>
       <c r="AM106" s="60">
         <f>(AM101*AM93)+(AM103*AM98)</f>
-        <v>8.0914998451780212E-2</v>
+        <v>8.08522976325073E-2</v>
       </c>
     </row>
     <row r="107" spans="1:39" ht="19" x14ac:dyDescent="0.25">
@@ -14766,7 +14768,7 @@
       <c r="AI108" s="44"/>
       <c r="AJ108" s="47">
         <f>AJ107*(1+AM108)/(AM109-AM108)</f>
-        <v>18881338267.592979</v>
+        <v>18902534806.11565</v>
       </c>
       <c r="AK108" s="48" t="s">
         <v>144</v>
@@ -14797,7 +14799,7 @@
       </c>
       <c r="AJ109" s="47">
         <f>AJ108+AJ107</f>
-        <v>19911338267.592979</v>
+        <v>19932534806.11565</v>
       </c>
       <c r="AK109" s="48" t="s">
         <v>142</v>
@@ -14807,7 +14809,7 @@
       </c>
       <c r="AM109" s="39">
         <f>AM106</f>
-        <v>8.0914998451780212E-2</v>
+        <v>8.08522976325073E-2</v>
       </c>
     </row>
     <row r="110" spans="1:39" ht="19" x14ac:dyDescent="0.2">
@@ -14828,7 +14830,7 @@
       </c>
       <c r="AG111" s="58">
         <f>NPV(AM109,AF109,AG109,AH109,AI109,AJ109)</f>
-        <v>15556494977.504606</v>
+        <v>15575114289.453318</v>
       </c>
       <c r="AH111" s="49"/>
       <c r="AI111" s="49"/>
@@ -14873,7 +14875,7 @@
       </c>
       <c r="AG114" s="58">
         <f>AG111+AG112-AG113</f>
-        <v>16602342977.504608</v>
+        <v>16620962289.453316</v>
       </c>
       <c r="AH114" s="49"/>
       <c r="AI114" s="49"/>
@@ -14903,7 +14905,7 @@
       </c>
       <c r="AG116" s="66">
         <f>AG114/AG115</f>
-        <v>39.646836647278903</v>
+        <v>39.691300059480142</v>
       </c>
       <c r="AH116" s="49"/>
       <c r="AI116" s="49"/>
@@ -14918,7 +14920,7 @@
       </c>
       <c r="AG117" s="67" cm="1">
         <f t="array" ref="AG117">_FV(A1,"Price")</f>
-        <v>52.36</v>
+        <v>52.65</v>
       </c>
       <c r="AH117" s="49"/>
       <c r="AI117" s="49"/>
@@ -14933,7 +14935,7 @@
       </c>
       <c r="AG118" s="68">
         <f>AG116/AG117-1</f>
-        <v>-0.24280296701148008</v>
+        <v>-0.24612915366609411</v>
       </c>
       <c r="AH118" s="49"/>
       <c r="AI118" s="49"/>

</xml_diff>

<commit_message>
Added new models and updates
</commit_message>
<xml_diff>
--- a/Commodities/Cameco.xlsx
+++ b/Commodities/Cameco.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Commodities/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/financial-modeling/Commodities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28203BDD-ACDF-7F40-8EE6-1838E15C6615}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91CFFB78-7AA8-E642-A0F4-601CC18FD602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2782,13 +2782,10 @@
       <sheetName val="Industrials"/>
       <sheetName val="Commodities"/>
       <sheetName val="US Treasury Bonds"/>
-      <sheetName val="Growth"/>
-      <sheetName val="Full Portfolio (Concentrated)"/>
-      <sheetName val="Value"/>
-      <sheetName val="Concentrated"/>
+      <sheetName val="High Growth"/>
+      <sheetName val="GARP"/>
       <sheetName val="Watchlist"/>
-      <sheetName val="Wide Moats"/>
-      <sheetName val="Sheet2"/>
+      <sheetName val="Highest Quality"/>
       <sheetName val="GARP HF Buys"/>
       <sheetName val="Value HF Buys"/>
       <sheetName val="Aggressive Growth HF Buys"/>
@@ -2805,7 +2802,7 @@
       <sheetData sheetId="7">
         <row r="8">
           <cell r="C8">
-            <v>4.845E-2</v>
+            <v>4.3360000000000003E-2</v>
           </cell>
         </row>
       </sheetData>
@@ -2817,9 +2814,6 @@
       <sheetData sheetId="13"/>
       <sheetData sheetId="14"/>
       <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2945,11 +2939,11 @@
     <v>268435456</v>
     <v>1</v>
     <v>Powered by Refinitiv</v>
-    <v>56.87</v>
+    <v>62.81</v>
     <v>28.98</v>
-    <v>0.92120000000000002</v>
-    <v>-0.38</v>
-    <v>-7.1660000000000005E-3</v>
+    <v>0.89459999999999995</v>
+    <v>-1.18</v>
+    <v>-1.9261999999999998E-2</v>
     <v>0</v>
     <v>0</v>
     <v>CAD</v>
@@ -2959,25 +2953,25 @@
     <v>XTSE</v>
     <v>XTSE</v>
     <v>2121 11th St W, SASKATOON, SK, S7M 1J3 CA</v>
-    <v>53.63</v>
+    <v>61.49</v>
     <v>Uranium</v>
     <v>Stock</v>
-    <v>45226.833333333336</v>
+    <v>45259.885763888888</v>
     <v>0</v>
-    <v>52.465000000000003</v>
-    <v>22904310000</v>
+    <v>59.84</v>
+    <v>26630660000</v>
     <v>CAMECO CORPORATION</v>
     <v>CAMECO CORPORATION</v>
-    <v>53.51</v>
-    <v>243.33</v>
-    <v>53.03</v>
-    <v>52.65</v>
-    <v>52.65</v>
-    <v>433837700</v>
+    <v>61.49</v>
+    <v>99.191000000000003</v>
+    <v>61.26</v>
+    <v>60.08</v>
+    <v>60.08</v>
+    <v>433865400</v>
     <v>CCO</v>
     <v>CAMECO CORPORATION (XTSE:CCO)</v>
-    <v>697591</v>
-    <v>1083790</v>
+    <v>1448162</v>
+    <v>821740</v>
     <v>1997</v>
   </rv>
   <rv s="2">
@@ -3563,10 +3557,10 @@
   <dimension ref="A1:AN119"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="AB95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="AB89" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="AF121" sqref="AF121"/>
+      <selection pane="bottomRight" activeCell="AF97" sqref="AF97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5380,15 +5374,15 @@
       </c>
       <c r="AL16" s="32">
         <f>AM102/AE3</f>
-        <v>12.261388231175218</v>
+        <v>14.256219074594634</v>
       </c>
       <c r="AM16" s="32">
         <f>AM102/AE28</f>
-        <v>256.2519299187756</v>
+        <v>297.94209124879728</v>
       </c>
       <c r="AN16" s="33">
         <f>AM102/AE107</f>
-        <v>142.12243808909213</v>
+        <v>165.2446341811503</v>
       </c>
     </row>
     <row r="17" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -5708,15 +5702,15 @@
       </c>
       <c r="AL19" s="32">
         <f>AM102/AF3</f>
-        <v>9.2880413625304143</v>
+        <v>10.799132197891321</v>
       </c>
       <c r="AM19" s="32">
         <f>AM102/AF28</f>
-        <v>76.989277310924365</v>
+        <v>89.514823529411771</v>
       </c>
       <c r="AN19" s="33">
         <f>AM102/AF107</f>
-        <v>96.236596638655456</v>
+        <v>111.8935294117647</v>
       </c>
     </row>
     <row r="20" spans="1:40" ht="19" customHeight="1" x14ac:dyDescent="0.25">
@@ -6085,11 +6079,11 @@
       </c>
       <c r="AM22" s="42">
         <f>(-1*AE98)/AM102</f>
-        <v>2.2657307729418612E-3</v>
+        <v>1.9486937237004264E-3</v>
       </c>
       <c r="AN22" s="41">
         <f>AF107/AM102</f>
-        <v>1.039105740360657E-2</v>
+        <v>8.9370672750881883E-3</v>
       </c>
     </row>
     <row r="23" spans="1:40" ht="19" x14ac:dyDescent="0.25">
@@ -7235,7 +7229,7 @@
       </c>
       <c r="AF33" s="1" cm="1">
         <f t="array" ref="AF33">_FV(A1,"Shares outstanding",TRUE)</f>
-        <v>433837700</v>
+        <v>433865400</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -7334,7 +7328,7 @@
       </c>
       <c r="AF34" s="1" cm="1">
         <f t="array" ref="AF34">_FV(A1,"Shares outstanding",TRUE)</f>
-        <v>433837700</v>
+        <v>433865400</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -7460,7 +7454,7 @@
       </c>
       <c r="AF35" s="22">
         <f t="shared" si="17"/>
-        <v>6.5586844658405682E-2</v>
+        <v>6.5654881059108161E-2</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="19" x14ac:dyDescent="0.25">
@@ -13367,7 +13361,7 @@
       </c>
       <c r="AM95" s="56">
         <f>'[1]US Treasury Bonds'!$C$8</f>
-        <v>4.845E-2</v>
+        <v>4.3360000000000003E-2</v>
       </c>
     </row>
     <row r="96" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -13475,7 +13469,7 @@
       </c>
       <c r="AM96" s="57" cm="1">
         <f t="array" ref="AM96">_FV(A1,"Beta")</f>
-        <v>0.92120000000000002</v>
+        <v>0.89459999999999995</v>
       </c>
     </row>
     <row r="97" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -13690,7 +13684,7 @@
       </c>
       <c r="AM98" s="55">
         <f>(AM95)+((AM96)*(AM97-AM95))</f>
-        <v>8.1198660000000006E-2</v>
+        <v>7.9716544E-2</v>
       </c>
     </row>
     <row r="99" spans="1:39" ht="20" customHeight="1" x14ac:dyDescent="0.25">
@@ -14011,7 +14005,7 @@
       </c>
       <c r="AM101" s="55">
         <f>AM100/AM104</f>
-        <v>4.1713194799782943E-2</v>
+        <v>3.6087022932814433E-2</v>
       </c>
     </row>
     <row r="102" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -14119,7 +14113,7 @@
       </c>
       <c r="AM102" s="58" cm="1">
         <f t="array" ref="AM102">_FV(A1,"Market cap",TRUE)</f>
-        <v>22904310000</v>
+        <v>26630660000</v>
       </c>
     </row>
     <row r="103" spans="1:39" ht="20" x14ac:dyDescent="0.25">
@@ -14227,7 +14221,7 @@
       </c>
       <c r="AM103" s="55">
         <f>AM102/AM104</f>
-        <v>0.95828680520021703</v>
+        <v>0.96391297706718559</v>
       </c>
     </row>
     <row r="104" spans="1:39" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -14337,7 +14331,7 @@
       </c>
       <c r="AM104" s="59">
         <f>AM100+AM102</f>
-        <v>23901310000</v>
+        <v>27627660000</v>
       </c>
     </row>
     <row r="105" spans="1:39" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -14638,7 +14632,7 @@
       </c>
       <c r="AM106" s="60">
         <f>(AM101*AM93)+(AM103*AM98)</f>
-        <v>8.08522976325073E-2</v>
+        <v>7.9470383280424869E-2</v>
       </c>
     </row>
     <row r="107" spans="1:39" ht="19" x14ac:dyDescent="0.25">
@@ -14768,7 +14762,7 @@
       <c r="AI108" s="44"/>
       <c r="AJ108" s="47">
         <f>AJ107*(1+AM108)/(AM109-AM108)</f>
-        <v>18902534806.11565</v>
+        <v>19382092366.869884</v>
       </c>
       <c r="AK108" s="48" t="s">
         <v>144</v>
@@ -14799,7 +14793,7 @@
       </c>
       <c r="AJ109" s="47">
         <f>AJ108+AJ107</f>
-        <v>19932534806.11565</v>
+        <v>20412092366.869884</v>
       </c>
       <c r="AK109" s="48" t="s">
         <v>142</v>
@@ -14809,7 +14803,7 @@
       </c>
       <c r="AM109" s="39">
         <f>AM106</f>
-        <v>8.08522976325073E-2</v>
+        <v>7.9470383280424869E-2</v>
       </c>
     </row>
     <row r="110" spans="1:39" ht="19" x14ac:dyDescent="0.2">
@@ -14830,7 +14824,7 @@
       </c>
       <c r="AG111" s="58">
         <f>NPV(AM109,AF109,AG109,AH109,AI109,AJ109)</f>
-        <v>15575114289.453318</v>
+        <v>15996425533.558701</v>
       </c>
       <c r="AH111" s="49"/>
       <c r="AI111" s="49"/>
@@ -14875,7 +14869,7 @@
       </c>
       <c r="AG114" s="58">
         <f>AG111+AG112-AG113</f>
-        <v>16620962289.453316</v>
+        <v>17042273533.558701</v>
       </c>
       <c r="AH114" s="49"/>
       <c r="AI114" s="49"/>
@@ -14905,7 +14899,7 @@
       </c>
       <c r="AG116" s="66">
         <f>AG114/AG115</f>
-        <v>39.691300059480142</v>
+        <v>40.697402517147758</v>
       </c>
       <c r="AH116" s="49"/>
       <c r="AI116" s="49"/>
@@ -14920,7 +14914,7 @@
       </c>
       <c r="AG117" s="67" cm="1">
         <f t="array" ref="AG117">_FV(A1,"Price")</f>
-        <v>52.65</v>
+        <v>60.08</v>
       </c>
       <c r="AH117" s="49"/>
       <c r="AI117" s="49"/>
@@ -14935,7 +14929,7 @@
       </c>
       <c r="AG118" s="68">
         <f>AG116/AG117-1</f>
-        <v>-0.24612915366609411</v>
+        <v>-0.32261314052683487</v>
       </c>
       <c r="AH118" s="49"/>
       <c r="AI118" s="49"/>

</xml_diff>